<commit_message>
Updated coding for App.java
</commit_message>
<xml_diff>
--- a/Adrien_1276832_Billy_1298073/10x10_Test_Template.xlsx
+++ b/Adrien_1276832_Billy_1298073/10x10_Test_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GGPC\Documents\Adrien Work\COMPX556\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GGPC\Documents\Adrien Work\COMPX556\Project\COMPX556_ACO_Parallelism\Adrien_1276832_Billy_1298073\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C7DE81-B1A2-4E7F-B7B9-C3E021EEBD21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7404EDC-5CC4-4576-8D19-EF4131BFB37F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,13 +414,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1">
         <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1">

</xml_diff>